<commit_message>
Implementation of Case_2 - Complete
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Logistic_Regression\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC203F6E-A72D-4910-923C-902D0424F034}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99122C63-A341-4A01-9FD9-576000C761F3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <author>Gabriel Hayat</author>
   </authors>
   <commentList>
-    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{1952DE88-0714-4F2D-9737-00B0C48DCD2E}">
+    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
       <text>
         <r>
           <rPr>
@@ -38,7 +38,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Gabriel Hayat:</t>
         </r>
@@ -47,15 +47,15 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-FMMMM, epoch
-In this model, cluster 0 contains the minority group. Thus, the cluster images are upsampled every epoch%5 == 0 during the training process</t>
+Here, a reweightring factor has been applied only the females earning more than &gt;50K. The new weight has been found by:
+n(Male earning &gt;50K)/n(Female earning &gt;50K)</t>
         </r>
       </text>
     </comment>
-    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{7E91B3F7-3220-437D-8D80-3B92B1320C0B}">
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
       <text>
         <r>
           <rPr>
@@ -63,32 +63,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Gabriel Hayat:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MMMMF, epoch
-In this model, cluster 4 contains the minority group. Thus, the cluster images are upsampled every epoch%5 == 4 during the training process</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{EE980B27-1331-4B99-966E-884188D075D5}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Gabriel Hayat:</t>
         </r>
@@ -97,86 +72,12 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-FMMMM, iteration
-Instead of upsampling the same cluster at every iteration, we upsample according to the batch index</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I15" authorId="0" shapeId="0" xr:uid="{FD973072-68AE-49D0-9870-8D80A77A8452}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Gabriel Hayat:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-FMMMM, epoch
-In this model, cluster 0 contains the minority group. Thus, the cluster images are upsampled every epoch%5 == 0 during the training process</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I16" authorId="0" shapeId="0" xr:uid="{6BB9AEB1-B723-4D8C-B1D3-63EF9C56E9FF}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Gabriel Hayat:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>MMMMF, epoch
-In this model, cluster 4 contains the minority group. Thus, the cluster images are upsampled every epoch%5 == 4 during the training process</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="I17" authorId="0" shapeId="0" xr:uid="{6B2994F5-DFAB-49E0-BF3C-4AAE12D11E89}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Gabriel Hayat:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-FMMMM, iteration
-Instead of upsampling the same cluster at every iteration, we upsample according to the batch index</t>
+Here, a reweightring factor has been applied to both the females earning more than &gt;50K and females earning &lt;50K. The new weights has been found by:
+n(male earning &gt;50K)/n(female earning &gt;50K)
+n(male earning &lt;50K)/n(female earning &lt;50K)</t>
         </r>
       </text>
     </comment>
@@ -185,7 +86,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
   <si>
     <t>Training acc</t>
   </si>
@@ -302,6 +203,105 @@
   </si>
   <si>
     <t>0.174</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_1\checkpoints\model_ep_40\Run_1</t>
+  </si>
+  <si>
+    <t>0.779 +/- 0.0008</t>
+  </si>
+  <si>
+    <t>0.786 +/- 0.0009</t>
+  </si>
+  <si>
+    <t>0.566 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.755 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.924 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.899 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.185</t>
+  </si>
+  <si>
+    <t>0.023</t>
+  </si>
+  <si>
+    <t>0.197</t>
+  </si>
+  <si>
+    <t>0.021</t>
+  </si>
+  <si>
+    <t>0.186</t>
+  </si>
+  <si>
+    <t>0.024</t>
+  </si>
+  <si>
+    <t>0.191</t>
+  </si>
+  <si>
+    <t>0.027</t>
+  </si>
+  <si>
+    <t>0.029</t>
+  </si>
+  <si>
+    <t>0.183</t>
+  </si>
+  <si>
+    <t>Case_2</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_1\checkpoints\model_ep_40\Run_2</t>
+  </si>
+  <si>
+    <t>0.792 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.796 +/- 0.0006</t>
+  </si>
+  <si>
+    <t>0.586 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.821 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.9162 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.864 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.238</t>
+  </si>
+  <si>
+    <t>0.051</t>
+  </si>
+  <si>
+    <t>0.231</t>
+  </si>
+  <si>
+    <t>0.053</t>
+  </si>
+  <si>
+    <t>0.054</t>
+  </si>
+  <si>
+    <t>0.052</t>
+  </si>
+  <si>
+    <t>0.235</t>
+  </si>
+  <si>
+    <t>0.239</t>
   </si>
 </sst>
 </file>
@@ -324,19 +324,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -349,6 +336,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -417,13 +417,13 @@
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -434,26 +434,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -741,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S18"/>
+  <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,26 +800,26 @@
       <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="J1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="15"/>
-      <c r="L1" s="13" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="13"/>
-      <c r="N1" s="12" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="12"/>
-      <c r="P1" s="13" t="s">
+      <c r="O1" s="13"/>
+      <c r="P1" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="12" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="12"/>
+      <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="5" t="s">
@@ -913,40 +916,123 @@
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="5"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
+      <c r="B4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N4" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="P4" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="S4" s="9" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="3"/>
+      <c r="A5" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" t="s">
+        <v>66</v>
+      </c>
+      <c r="M5" t="s">
+        <v>67</v>
+      </c>
+      <c r="N5" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="O5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="R5" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="S5" s="11" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="3"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B7" s="14">
         <v>4</v>
-      </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B7" s="14">
-        <v>5</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
@@ -956,28 +1042,29 @@
       <c r="H7" s="14"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="15">
+        <v>5</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="13" t="s">
+    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="5"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9"/>
-      <c r="R9" s="9"/>
-      <c r="S9" s="9"/>
-    </row>
-    <row r="10" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="13"/>
+      <c r="C10" s="1"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5"/>
       <c r="G10" s="4"/>
@@ -990,9 +1077,7 @@
       <c r="S10" s="9"/>
     </row>
     <row r="11" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
-      </c>
+      <c r="A11" s="14"/>
       <c r="E11" s="4"/>
       <c r="F11" s="5"/>
       <c r="G11" s="4"/>
@@ -1004,43 +1089,45 @@
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
     </row>
-    <row r="12" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="10" t="s">
+    <row r="12" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="5"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B14" s="15">
         <v>2</v>
       </c>
-      <c r="C13" s="14"/>
-      <c r="D13" s="14"/>
-      <c r="E13" s="14"/>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="13" t="s">
+    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="5"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="9"/>
-      <c r="R15" s="9"/>
-      <c r="S15" s="9"/>
-    </row>
-    <row r="16" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="13"/>
       <c r="E16" s="4"/>
       <c r="F16" s="5"/>
       <c r="G16" s="4"/>
@@ -1049,13 +1136,11 @@
       <c r="K16" s="9"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
     </row>
     <row r="17" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="7" t="s">
-        <v>7</v>
-      </c>
+      <c r="A17" s="14"/>
       <c r="E17" s="4"/>
       <c r="F17" s="5"/>
       <c r="G17" s="4"/>
@@ -1064,22 +1149,37 @@
       <c r="K17" s="9"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
-      <c r="R17" s="9"/>
-      <c r="S17" s="9"/>
-    </row>
-    <row r="18" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="R17" s="11"/>
+      <c r="S17" s="11"/>
+    </row>
+    <row r="18" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="5"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B14:H14"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A10:A11"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
+    <mergeCell ref="B8:H8"/>
     <mergeCell ref="B7:H7"/>
-    <mergeCell ref="B6:H6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Sample features now contain gender attribute
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF774DD0-0BAB-4388-BDA3-69CAB7583984}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9D3FB7E-06F1-4A99-9CF6-B6D13CF5D2FF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,31 @@
     <author>Gabriel Hayat</author>
   </authors>
   <commentList>
-    <comment ref="I4" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
+    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{853C7786-0175-49FB-A01E-8E1EA80AE0B4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In the following three cases, the features of training data don't contain the protected attribute. In other words, the model does not have access to the senstitive attribute when training.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
       <text>
         <r>
           <rPr>
@@ -55,7 +79,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
+    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
       <text>
         <r>
           <rPr>
@@ -81,12 +105,61 @@
         </r>
       </text>
     </comment>
+    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{B1B0EECE-82BA-4961-B120-51E80FE68B69}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+In the following three cases, the sensitive attribute is part of the features of the training data, thus the model has access to the sensitive attribute when training.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{945AFF0F-7AF8-484B-A291-F2DE81F22AC9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Here, a reweightring factor has been applied only the females earning more than &gt;50K. The new weight has been found by:
+n(Male earning &gt;50K)/n(Female earning &gt;50K)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
   <si>
     <t>Training acc</t>
   </si>
@@ -103,9 +176,6 @@
     <t>Case 1</t>
   </si>
   <si>
-    <t>Case 2</t>
-  </si>
-  <si>
     <t>Case 3 - Epoch</t>
   </si>
   <si>
@@ -253,12 +323,6 @@
     <t>0.183</t>
   </si>
   <si>
-    <t>Case_2</t>
-  </si>
-  <si>
-    <t>0.792 +/- 0.003</t>
-  </si>
-  <si>
     <t>0.796 +/- 0.0006</t>
   </si>
   <si>
@@ -302,6 +366,108 @@
   </si>
   <si>
     <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_2\checkpoints\model_ep_40\Run_1</t>
+  </si>
+  <si>
+    <t>0.792 +/- 0.0003</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_1\checkpoints\model_ep_40\Run_1</t>
+  </si>
+  <si>
+    <t>0.801 +/- 0.0007</t>
+  </si>
+  <si>
+    <t>0.774 +/- 0.0018</t>
+  </si>
+  <si>
+    <t>0.664 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.935 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.884 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.646 +/- 0.008</t>
+  </si>
+  <si>
+    <t>0.299</t>
+  </si>
+  <si>
+    <t>0.224</t>
+  </si>
+  <si>
+    <t>0.301</t>
+  </si>
+  <si>
+    <t>0.242</t>
+  </si>
+  <si>
+    <t>0.309</t>
+  </si>
+  <si>
+    <t>0.251</t>
+  </si>
+  <si>
+    <t>0.293</t>
+  </si>
+  <si>
+    <t>0.232</t>
+  </si>
+  <si>
+    <t>0.302</t>
+  </si>
+  <si>
+    <t>0.244</t>
+  </si>
+  <si>
+    <t>Case 2 a.</t>
+  </si>
+  <si>
+    <t>Case 2 b.</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_2\checkpoints\model_ep_40\Run_2</t>
+  </si>
+  <si>
+    <t>0.790 +/- 0.0005</t>
+  </si>
+  <si>
+    <t>0.797 +/- 0.0018</t>
+  </si>
+  <si>
+    <t>0.616 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.79 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.902 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.882 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.176</t>
+  </si>
+  <si>
+    <t>0.019</t>
+  </si>
+  <si>
+    <t>0.022</t>
+  </si>
+  <si>
+    <t>0.177</t>
+  </si>
+  <si>
+    <t>0.018</t>
+  </si>
+  <si>
+    <t>0.178</t>
+  </si>
+  <si>
+    <t>0.17</t>
   </si>
 </sst>
 </file>
@@ -431,9 +597,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
@@ -444,6 +607,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -744,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S19"/>
+  <dimension ref="A1:S22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -773,8 +939,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="6" t="s">
-        <v>8</v>
+      <c r="A1" s="5" t="s">
+        <v>7</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
@@ -783,402 +949,533 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="5" t="s">
-        <v>25</v>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="16"/>
       <c r="L1" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M1" s="14"/>
       <c r="N1" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O1" s="13"/>
       <c r="P1" s="14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Q1" s="14"/>
       <c r="R1" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S1" s="13"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="8" t="s">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="7" t="s">
         <v>22</v>
       </c>
+      <c r="K2" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="L2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="M2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="N2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="O2" s="8" t="s">
+      <c r="O2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" t="s">
         <v>22</v>
       </c>
-      <c r="P2" t="s">
-        <v>23</v>
-      </c>
       <c r="Q2" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="R2" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="S2" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="K3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L3" t="s">
-        <v>37</v>
-      </c>
-      <c r="M3" t="s">
-        <v>38</v>
-      </c>
-      <c r="N3" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="O3" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="P3" s="11" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q3" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>17</v>
-      </c>
+      <c r="S2" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" t="s">
+        <v>36</v>
+      </c>
+      <c r="M4" t="s">
+        <v>37</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q4" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" t="s">
         <v>39</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E5" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F5" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="G5" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="J5" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="K5" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="K4" s="8" t="s">
+      <c r="L5" t="s">
         <v>46</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M5" t="s">
+        <v>52</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="O5" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="M4" t="s">
-        <v>53</v>
-      </c>
-      <c r="N4" s="9" t="s">
+      <c r="P5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="P4" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="R4" s="9" t="s">
-        <v>51</v>
-      </c>
-      <c r="S4" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="E6" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="F6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D5" t="s">
+      <c r="G6" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="E5" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="J6" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="K6" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="L6" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="M6" t="s">
         <v>62</v>
       </c>
-      <c r="K5" s="11" t="s">
+      <c r="N6" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="O6" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="L5" t="s">
+      <c r="P6" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="M5" t="s">
+      <c r="R6" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="N5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="O5" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="P5" s="11" t="s">
+      <c r="S6" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="Q5" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="R5" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="S5" s="11" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="3"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" s="14">
-        <v>4</v>
-      </c>
+      <c r="A7" s="12"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="14"/>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A8" s="10" t="s">
+      <c r="I7" s="12"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" t="s">
+        <v>72</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="J8" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="L8" t="s">
+        <v>79</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+      <c r="N8" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="P8" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>84</v>
+      </c>
+      <c r="R8" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" t="s">
+        <v>90</v>
+      </c>
+      <c r="D9" t="s">
+        <v>91</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="J9" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="K9" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="L9" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" t="s">
+        <v>98</v>
+      </c>
+      <c r="N9" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="O9" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="R9" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B10" s="14">
+        <v>4</v>
+      </c>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="15">
         <v>5</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="14" t="s">
+    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="4"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="R13" s="8"/>
+      <c r="S13" s="8"/>
+    </row>
+    <row r="14" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="14"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="4"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="R14" s="8"/>
+      <c r="S14" s="8"/>
+    </row>
+    <row r="15" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="5"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-      <c r="R10" s="9"/>
-      <c r="S10" s="9"/>
-    </row>
-    <row r="11" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="14"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="5"/>
-      <c r="J11" s="9"/>
-      <c r="K11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
-      <c r="R11" s="9"/>
-      <c r="S11" s="9"/>
-    </row>
-    <row r="12" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E12" s="4"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="5"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="R12" s="9"/>
-      <c r="S12" s="9"/>
-    </row>
-    <row r="13" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B14" s="15">
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="4"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="R15" s="8"/>
+      <c r="S15" s="8"/>
+    </row>
+    <row r="16" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" s="15">
         <v>2</v>
       </c>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
-      <c r="G14" s="15"/>
-      <c r="H14" s="15"/>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="C17" s="15"/>
+      <c r="D17" s="15"/>
+      <c r="E17" s="15"/>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A16" s="14" t="s">
+    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="4"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="R19" s="8"/>
+      <c r="S19" s="8"/>
+    </row>
+    <row r="20" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A20" s="14"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="4"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="N20" s="8"/>
+      <c r="O20" s="8"/>
+      <c r="R20" s="10"/>
+      <c r="S20" s="10"/>
+    </row>
+    <row r="21" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A21" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="E16" s="4"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="4"/>
-      <c r="H16" s="5"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="9"/>
-      <c r="R16" s="9"/>
-      <c r="S16" s="9"/>
-    </row>
-    <row r="17" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="14"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="5"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-    </row>
-    <row r="18" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="9"/>
-      <c r="R18" s="9"/>
-      <c r="S18" s="9"/>
-    </row>
-    <row r="19" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="4"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="N21" s="8"/>
+      <c r="O21" s="8"/>
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+    </row>
+    <row r="22" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="12">
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="B14:H14"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B17:H17"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A13:A14"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B8:H8"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B10:H10"/>
+    <mergeCell ref="B3:H3"/>
     <mergeCell ref="B7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Results of dummy Case_3
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC6DF711-EBBE-4CD5-B313-F703E5AE6F89}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B262E0E-8134-4286-B2BC-CBAB6836C45F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -129,12 +129,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{54CBADAE-66FB-43A8-9458-E34F3EB4A4A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+First attempt at updating cluster weights at each epoch. Here, there are two clusters (M, F) for each label. The dommy update rule of the cluster weights is the following one: 
+w_cluster += avg_accuracy(clusters of same label) - accuracy(cluster)
+if w_cluster &lt; 1: w_cluster = 1</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
   <si>
     <t>Training acc</t>
   </si>
@@ -142,21 +168,12 @@
     <t>Note</t>
   </si>
   <si>
-    <t>Upweighting technique</t>
-  </si>
-  <si>
     <t>Path</t>
   </si>
   <si>
     <t>Case 1</t>
   </si>
   <si>
-    <t>Case 3 - Epoch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Case 3 - Iteration </t>
-  </si>
-  <si>
     <t>MALE</t>
   </si>
   <si>
@@ -187,12 +204,6 @@
     <t>0.166</t>
   </si>
   <si>
-    <t xml:space="preserve">number of clusters </t>
-  </si>
-  <si>
-    <t>Reweighting ratio</t>
-  </si>
-  <si>
     <t>Test acc</t>
   </si>
   <si>
@@ -443,23 +454,67 @@
   </si>
   <si>
     <t>0.17</t>
+  </si>
+  <si>
+    <t>Case 3</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_0</t>
+  </si>
+  <si>
+    <t>0.789 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.797 +/- 0-0049</t>
+  </si>
+  <si>
+    <t>0.773 +/- 0.019</t>
+  </si>
+  <si>
+    <t>0.863 +/- 0.016</t>
+  </si>
+  <si>
+    <t>0.752 +/- 0.026</t>
+  </si>
+  <si>
+    <t>0.801 +/- 0.027</t>
+  </si>
+  <si>
+    <t>0.092</t>
+  </si>
+  <si>
+    <t>0.0092</t>
+  </si>
+  <si>
+    <t>0.05</t>
+  </si>
+  <si>
+    <t>0.084</t>
+  </si>
+  <si>
+    <t>0.044</t>
+  </si>
+  <si>
+    <t>0.086</t>
+  </si>
+  <si>
+    <t>0.043</t>
+  </si>
+  <si>
+    <t>0.096</t>
+  </si>
+  <si>
+    <t>0.049</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -492,7 +547,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -519,12 +574,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -556,53 +605,44 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="6">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="20% - Accent6" xfId="5" builtinId="50"/>
+  <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
@@ -885,10 +925,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S22"/>
+  <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -914,542 +954,482 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="5" t="s">
-        <v>7</v>
+      <c r="A1" s="4" t="s">
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>19</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>24</v>
       </c>
       <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="J1" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="12"/>
+      <c r="L1" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="O1" s="10"/>
+      <c r="P1" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="14" t="s">
+      <c r="Q1" s="11"/>
+      <c r="R1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="13" t="s">
+      <c r="S1" s="10"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="L2" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>16</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="B3" s="11"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="13"/>
-      <c r="P1" s="14" t="s">
+      <c r="L4" t="s">
+        <v>31</v>
+      </c>
+      <c r="M4" t="s">
+        <v>32</v>
+      </c>
+      <c r="N4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="13" t="s">
+      <c r="O4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="13"/>
-    </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" t="s">
-        <v>22</v>
-      </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="O2" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-    </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="P4" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="S4" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="L5" t="s">
+        <v>41</v>
+      </c>
+      <c r="M5" t="s">
+        <v>47</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>44</v>
+      </c>
+      <c r="R5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J6" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="K6" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L6" t="s">
+        <v>56</v>
+      </c>
+      <c r="M6" t="s">
+        <v>57</v>
+      </c>
+      <c r="N6" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="O6" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="P6" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>59</v>
+      </c>
+      <c r="R6" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="S6" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="9"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C8" t="s">
+        <v>66</v>
+      </c>
+      <c r="D8" t="s">
+        <v>67</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="K8" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="L8" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="P8" t="s">
+        <v>78</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>79</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="S8" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
+        <v>85</v>
+      </c>
+      <c r="D9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="L9" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="L4" t="s">
-        <v>36</v>
-      </c>
-      <c r="M4" t="s">
-        <v>37</v>
-      </c>
-      <c r="N4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="P4" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="R4" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="G5" s="3" t="s">
+      <c r="M9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P9" t="s">
+        <v>96</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>92</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="S9" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="H5" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="K5" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" t="s">
-        <v>46</v>
-      </c>
-      <c r="M5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="R5" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="S5" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B6" t="s">
-        <v>68</v>
-      </c>
-      <c r="C6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D6" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="H6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="J6" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="K6" s="10" t="s">
-        <v>60</v>
-      </c>
-      <c r="L6" t="s">
-        <v>61</v>
-      </c>
-      <c r="M6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N6" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="O6" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="P6" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q6" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="R6" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="S6" s="10" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="12"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="12"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" t="s">
-        <v>70</v>
-      </c>
-      <c r="C8" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" t="s">
-        <v>72</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K8" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="L8" t="s">
-        <v>79</v>
-      </c>
-      <c r="M8" t="s">
-        <v>80</v>
-      </c>
-      <c r="N8" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="O8" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="P8" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>84</v>
-      </c>
-      <c r="R8" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="S8" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="B9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C9" t="s">
-        <v>90</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="K9" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="L9" t="s">
-        <v>35</v>
-      </c>
-      <c r="M9" t="s">
-        <v>98</v>
-      </c>
-      <c r="N9" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="O9" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="P9" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="Q9" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="R9" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="S9" s="8" t="s">
-        <v>47</v>
-      </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="14">
-        <v>4</v>
-      </c>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="15">
-        <v>5</v>
-      </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="15"/>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="4"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
-      <c r="N13" s="8"/>
-      <c r="O13" s="8"/>
-      <c r="R13" s="8"/>
-      <c r="S13" s="8"/>
-    </row>
-    <row r="14" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="14"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="4"/>
-      <c r="J14" s="8"/>
-      <c r="K14" s="8"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="8"/>
-      <c r="R14" s="8"/>
-      <c r="S14" s="8"/>
-    </row>
-    <row r="15" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="4"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="8"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
-    </row>
-    <row r="16" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A17" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="15">
-        <v>2</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="15"/>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="3"/>
-      <c r="H19" s="4"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="8"/>
-    </row>
-    <row r="20" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="14"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="4"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="8"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
-    </row>
-    <row r="21" spans="1:19" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="4"/>
-      <c r="J21" s="8"/>
-      <c r="K21" s="8"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-    </row>
-    <row r="22" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+        <v>98</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="F11" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="H11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="J11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" t="s">
+        <v>107</v>
+      </c>
+      <c r="M11" t="s">
+        <v>108</v>
+      </c>
+      <c r="N11" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="P11" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>112</v>
+      </c>
+      <c r="R11" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="13"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="13"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B17" s="13"/>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19" s="13"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" s="13"/>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="7">
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
-    <mergeCell ref="B17:H17"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A13:A14"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B10:H10"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="B7:H7"/>
   </mergeCells>

</xml_diff>

<commit_message>
Cluster weights gradient ascent - implementation complete
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B262E0E-8134-4286-B2BC-CBAB6836C45F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13380F37-2B25-4C14-8B74-A9655967DB74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -155,12 +155,38 @@
         </r>
       </text>
     </comment>
+    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{07BB9D53-FAF3-410B-B71D-53A991FB2529}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Here, the weights are updated after each batch of each epoch, by performing gradient_ascent. Note the learning rate of the weight updates is not optimized and might not be appropriate for the current number of epochs (40)
+Note: + the standart deviation is a lot smaller than case a), meaning the approach is more stable. 
+         - problem with this approach is that even the weights of the clusters with high accuracy keep increasing since their gradient is not exactly 0.</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="130">
   <si>
     <t>Training acc</t>
   </si>
@@ -456,9 +482,6 @@
     <t>0.17</t>
   </si>
   <si>
-    <t>Case 3</t>
-  </si>
-  <si>
     <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_0</t>
   </si>
   <si>
@@ -505,6 +528,54 @@
   </si>
   <si>
     <t>0.049</t>
+  </si>
+  <si>
+    <t>Case 3 a.</t>
+  </si>
+  <si>
+    <t>Case 3 b.</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_1</t>
+  </si>
+  <si>
+    <t>0.805 +/- 0.000</t>
+  </si>
+  <si>
+    <t>0.794 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.697 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.895 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.838 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.748 +/- 0.005</t>
+  </si>
+  <si>
+    <t>0.2</t>
+  </si>
+  <si>
+    <t>0.098</t>
+  </si>
+  <si>
+    <t>0.201</t>
+  </si>
+  <si>
+    <t>0.091</t>
+  </si>
+  <si>
+    <t>0.192</t>
+  </si>
+  <si>
+    <t>0.081</t>
+  </si>
+  <si>
+    <t>0.09</t>
   </si>
 </sst>
 </file>
@@ -612,7 +683,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -629,6 +700,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,9 +715,6 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
@@ -928,7 +1002,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="O29" sqref="O28:O29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -981,26 +1055,26 @@
       <c r="I1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="J1" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="12"/>
-      <c r="L1" s="11" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="10" t="s">
+      <c r="M1" s="15"/>
+      <c r="N1" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="11" t="s">
+      <c r="O1" s="14"/>
+      <c r="P1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="10" t="s">
+      <c r="Q1" s="15"/>
+      <c r="R1" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="10"/>
+      <c r="S1" s="14"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -1038,13 +1112,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -1216,13 +1290,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -1338,100 +1412,156 @@
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B11" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="D11" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="E11" s="12" t="s">
         <v>101</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="G11" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="H11" s="13" t="s">
         <v>104</v>
       </c>
-      <c r="H11" s="15" t="s">
+      <c r="J11" s="7" t="s">
         <v>105</v>
-      </c>
-      <c r="J11" s="7" t="s">
-        <v>106</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>55</v>
       </c>
       <c r="L11" t="s">
+        <v>106</v>
+      </c>
+      <c r="M11" t="s">
         <v>107</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="N11" s="7" t="s">
+      <c r="O11" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="O11" s="7" t="s">
+      <c r="P11" t="s">
         <v>110</v>
       </c>
-      <c r="P11" t="s">
+      <c r="Q11" t="s">
         <v>111</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" s="7" t="s">
         <v>112</v>
       </c>
-      <c r="R11" s="7" t="s">
+      <c r="S11" s="7" t="s">
         <v>113</v>
       </c>
-      <c r="S11" s="7" t="s">
-        <v>114</v>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="H12" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="L12" t="s">
+        <v>125</v>
+      </c>
+      <c r="M12" t="s">
+        <v>105</v>
+      </c>
+      <c r="N12" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="P12" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>128</v>
+      </c>
+      <c r="R12" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="13"/>
+      <c r="A13" s="11"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="11"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
+      <c r="A19" s="11"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
+      <c r="A20" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="B7:H7"/>
     <mergeCell ref="N1:O1"/>
     <mergeCell ref="P1:Q1"/>
     <mergeCell ref="R1:S1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="L1:M1"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Development measures of training process are now accessible
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13380F37-2B25-4C14-8B74-A9655967DB74}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF70EE-CE40-40A3-838E-08133AE6BF4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -177,7 +177,7 @@
           <t xml:space="preserve">
 Here, the weights are updated after each batch of each epoch, by performing gradient_ascent. Note the learning rate of the weight updates is not optimized and might not be appropriate for the current number of epochs (40)
 Note: + the standart deviation is a lot smaller than case a), meaning the approach is more stable. 
-         - problem with this approach is that even the weights of the clusters with high accuracy keep increasing since their gradient is not exactly 0.</t>
+         - problem with this approach is that even the weights of the clusters with high accuracy          keep increasing since their gradient is not exactly 0. This is the difference with Case 3 a, where only the weight of the clusters with low accuracy increased </t>
         </r>
       </text>
     </comment>
@@ -706,10 +706,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1002,7 +1002,7 @@
   <dimension ref="A1:S20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O29" sqref="O28:O29"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,22 +1059,22 @@
         <v>6</v>
       </c>
       <c r="K1" s="16"/>
-      <c r="L1" s="15" t="s">
+      <c r="L1" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="14" t="s">
+      <c r="M1" s="14"/>
+      <c r="N1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="15" t="s">
+      <c r="O1" s="15"/>
+      <c r="P1" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="14" t="s">
+      <c r="Q1" s="14"/>
+      <c r="R1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="14"/>
+      <c r="S1" s="15"/>
     </row>
     <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
@@ -1112,13 +1112,13 @@
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="15"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="14"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="1" t="s">
@@ -1290,13 +1290,13 @@
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="14"/>
+      <c r="D7" s="14"/>
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="9"/>
     </row>
     <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
New cluster weight update heuristic - New experiments - Added documentation
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBF70EE-CE40-40A3-838E-08133AE6BF4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BAF90F-7A1A-4CE2-B17F-047CEFAB9538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -30,7 +39,7 @@
     <author>Gabriel Hayat</author>
   </authors>
   <commentList>
-    <comment ref="B3" authorId="0" shapeId="0" xr:uid="{853C7786-0175-49FB-A01E-8E1EA80AE0B4}">
+    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{853C7786-0175-49FB-A01E-8E1EA80AE0B4}">
       <text>
         <r>
           <rPr>
@@ -54,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
+    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
       <text>
         <r>
           <rPr>
@@ -79,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
       <text>
         <r>
           <rPr>
@@ -105,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B7" authorId="0" shapeId="0" xr:uid="{B1B0EECE-82BA-4961-B120-51E80FE68B69}">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{B1B0EECE-82BA-4961-B120-51E80FE68B69}">
       <text>
         <r>
           <rPr>
@@ -129,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{54CBADAE-66FB-43A8-9458-E34F3EB4A4A1}">
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{54CBADAE-66FB-43A8-9458-E34F3EB4A4A1}">
       <text>
         <r>
           <rPr>
@@ -155,7 +164,59 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0" shapeId="0" xr:uid="{07BB9D53-FAF3-410B-B71D-53A991FB2529}">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{3F5E49D1-8C77-466D-AB69-2E3A4F4FEB46}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This trial is called Case 3. Cheat as it cheats into taking the weights from the last epoch of Case 3.a, and train the model from scatch with them. This experiment was useful to do because:
+-&gt; If better results, means training case3a for longer leads to better results
+-&gt; If worse, means that training model for longer will not really make a difference</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{07BB9D53-FAF3-410B-B71D-53A991FB2529}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Here, the weights are updated after each batch of each epoch, by performing gradient_ascent. Note the learning rate of the weight updates is not optimized and might not be appropriate for the current number of epochs (40)
+Note: + the standart deviation is a lot smaller than case a), meaning the approach is more stable. 
+         - problem with this approach is that even the weights of the clusters with high accuracy          keep increasing since their gradient is not exactly 0. This is the difference with Case 3 a, where only the weight of the clusters with low accuracy increased </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{E92869DF-B279-4286-B130-8DBDA1241BD0}">
       <text>
         <r>
           <rPr>
@@ -186,7 +247,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="170">
   <si>
     <t>Training acc</t>
   </si>
@@ -488,9 +549,6 @@
     <t>0.789 +/- 0.004</t>
   </si>
   <si>
-    <t>0.797 +/- 0-0049</t>
-  </si>
-  <si>
     <t>0.773 +/- 0.019</t>
   </si>
   <si>
@@ -506,9 +564,6 @@
     <t>0.092</t>
   </si>
   <si>
-    <t>0.0092</t>
-  </si>
-  <si>
     <t>0.05</t>
   </si>
   <si>
@@ -576,6 +631,132 @@
   </si>
   <si>
     <t>0.09</t>
+  </si>
+  <si>
+    <t>Case 3. Cheat</t>
+  </si>
+  <si>
+    <t>0.797 +/- 0.0049</t>
+  </si>
+  <si>
+    <t>0.767 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.862 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.756 +/- 0.006</t>
+  </si>
+  <si>
+    <t>0.800 +/- 0.007</t>
+  </si>
+  <si>
+    <t>0.789  +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.796 +/. 0.002</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_4</t>
+  </si>
+  <si>
+    <t>Case 3 c.</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_5</t>
+  </si>
+  <si>
+    <t>0.796 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.783 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.0748 +/- 0.007</t>
+  </si>
+  <si>
+    <t>0.912 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.783 +/- 0.009</t>
+  </si>
+  <si>
+    <t>0.691 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.172</t>
+  </si>
+  <si>
+    <t>0.175</t>
+  </si>
+  <si>
+    <t>0.106</t>
+  </si>
+  <si>
+    <t>0.168</t>
+  </si>
+  <si>
+    <t>0.078</t>
+  </si>
+  <si>
+    <t>0.158</t>
+  </si>
+  <si>
+    <t>40 epochs</t>
+  </si>
+  <si>
+    <t>160 epochs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Case 3c. </t>
+  </si>
+  <si>
+    <t>0.805 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.806 +/- 0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.745 +/- 0.003 </t>
+  </si>
+  <si>
+    <t>0.877 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.799 +/- 0.005</t>
+  </si>
+  <si>
+    <t>0.803 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.13</t>
+  </si>
+  <si>
+    <t>0.002</t>
+  </si>
+  <si>
+    <t>0.132</t>
+  </si>
+  <si>
+    <t>0.006</t>
+  </si>
+  <si>
+    <t>0.134</t>
+  </si>
+  <si>
+    <t>0.004</t>
+  </si>
+  <si>
+    <t>0.124</t>
+  </si>
+  <si>
+    <t>0.003</t>
+  </si>
+  <si>
+    <t>0.129</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_160\Run_0</t>
   </si>
 </sst>
 </file>
@@ -683,7 +864,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -706,6 +887,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -999,569 +1183,728 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S20"/>
+  <dimension ref="A1:T21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
-    <col min="4" max="4" width="17.453125" customWidth="1"/>
-    <col min="5" max="5" width="18.08984375" customWidth="1"/>
-    <col min="6" max="6" width="16.6328125" customWidth="1"/>
-    <col min="7" max="7" width="15.453125" customWidth="1"/>
-    <col min="8" max="8" width="16.453125" customWidth="1"/>
-    <col min="9" max="9" width="18.54296875" customWidth="1"/>
-    <col min="10" max="10" width="13.26953125" customWidth="1"/>
-    <col min="11" max="12" width="12.81640625" customWidth="1"/>
-    <col min="13" max="13" width="13.1796875" customWidth="1"/>
-    <col min="14" max="14" width="12.7265625" customWidth="1"/>
-    <col min="15" max="15" width="12.453125" customWidth="1"/>
-    <col min="16" max="16" width="12.54296875" customWidth="1"/>
-    <col min="17" max="17" width="12.7265625" customWidth="1"/>
-    <col min="18" max="18" width="12.90625" customWidth="1"/>
-    <col min="19" max="19" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="29" customWidth="1"/>
+    <col min="3" max="3" width="16.453125" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" customWidth="1"/>
+    <col min="5" max="5" width="17.453125" customWidth="1"/>
+    <col min="6" max="6" width="18.08984375" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="15.453125" customWidth="1"/>
+    <col min="9" max="9" width="16.453125" customWidth="1"/>
+    <col min="10" max="10" width="18.54296875" customWidth="1"/>
+    <col min="11" max="11" width="13.26953125" customWidth="1"/>
+    <col min="12" max="13" width="12.81640625" customWidth="1"/>
+    <col min="14" max="14" width="13.1796875" customWidth="1"/>
+    <col min="15" max="15" width="12.7265625" customWidth="1"/>
+    <col min="16" max="16" width="12.453125" customWidth="1"/>
+    <col min="17" max="17" width="12.54296875" customWidth="1"/>
+    <col min="18" max="18" width="12.7265625" customWidth="1"/>
+    <col min="19" max="19" width="12.90625" customWidth="1"/>
+    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="16" t="s">
+      <c r="K1" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="16"/>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="17"/>
+      <c r="M1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="14"/>
-      <c r="N1" s="15" t="s">
+      <c r="N1" s="15"/>
+      <c r="O1" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="15"/>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="16"/>
+      <c r="Q1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="15" t="s">
+      <c r="R1" s="15"/>
+      <c r="S1" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="15"/>
+      <c r="T1" s="16"/>
     </row>
-    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>17</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>16</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B3" s="14"/>
-      <c r="C3" s="14"/>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
     </row>
-    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="15" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>18</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>22</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>31</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>32</v>
       </c>
-      <c r="N4" s="6" t="s">
+      <c r="O4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="P4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="6" t="s">
+      <c r="S4" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S4" s="6" t="s">
+      <c r="T4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="1" t="s">
+    <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15"/>
+      <c r="B5" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>62</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>33</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="G5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>41</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>47</v>
       </c>
-      <c r="N5" s="6" t="s">
+      <c r="O5" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="P5" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>43</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>44</v>
       </c>
-      <c r="R5" s="6" t="s">
+      <c r="S5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="T5" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A6" s="15"/>
+      <c r="B6" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>63</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>64</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="L6" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>56</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="7" t="s">
+      <c r="O6" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>56</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>59</v>
       </c>
-      <c r="R6" s="7" t="s">
+      <c r="S6" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="T6" s="7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A7" s="9"/>
-      <c r="B7" s="14"/>
-      <c r="C7" s="14"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="9"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A7" s="15"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="9"/>
     </row>
-    <row r="8" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A8" s="15"/>
+      <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>65</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G8" s="2" t="s">
+      <c r="H8" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="L8" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>74</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>75</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="O8" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="P8" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>78</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>79</v>
       </c>
-      <c r="R8" s="6" t="s">
+      <c r="S8" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="T8" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="15"/>
+      <c r="B9" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>84</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>85</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>86</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>30</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>93</v>
       </c>
-      <c r="N9" s="6" t="s">
+      <c r="O9" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="P9" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>96</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>92</v>
       </c>
-      <c r="R9" s="6" t="s">
+      <c r="S9" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="T9" s="6" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B10" s="11"/>
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A10" s="15"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
       <c r="G10" s="11"/>
       <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A11" s="15"/>
+      <c r="B11" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M11" t="s">
+        <v>104</v>
+      </c>
+      <c r="N11" t="s">
+        <v>105</v>
+      </c>
+      <c r="O11" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="P11" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>108</v>
+      </c>
+      <c r="R11" t="s">
+        <v>109</v>
+      </c>
+      <c r="S11" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T11" s="7" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A12" s="15"/>
+      <c r="B12" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="H12" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="K12" s="7"/>
+      <c r="L12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A13" s="15"/>
+      <c r="B13" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="B11" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="G11" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="H11" s="13" t="s">
+      <c r="D13" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="K13" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="L13" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="M13" t="s">
+        <v>123</v>
+      </c>
+      <c r="N13" t="s">
         <v>104</v>
       </c>
-      <c r="J11" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="L11" t="s">
+      <c r="O13" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>125</v>
+      </c>
+      <c r="R13" t="s">
+        <v>126</v>
+      </c>
+      <c r="S13" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="T13" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A14" s="15"/>
+      <c r="B14" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="C14" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>139</v>
+      </c>
+      <c r="E14" t="s">
+        <v>140</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>141</v>
+      </c>
+      <c r="G14" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="H14" s="12" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="K14" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="L14" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="M14" t="s">
+        <v>146</v>
+      </c>
+      <c r="N14" t="s">
+        <v>147</v>
+      </c>
+      <c r="O14" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P14" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>148</v>
+      </c>
+      <c r="R14" t="s">
+        <v>149</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>150</v>
+      </c>
+      <c r="T14" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="M11" t="s">
-        <v>107</v>
-      </c>
-      <c r="N11" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="P11" t="s">
-        <v>110</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>111</v>
-      </c>
-      <c r="R11" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>113</v>
-      </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A12" s="10" t="s">
-        <v>115</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="C12" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="F12" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="H12" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="K12" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="L12" t="s">
-        <v>125</v>
-      </c>
-      <c r="M12" t="s">
-        <v>105</v>
-      </c>
-      <c r="N12" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O12" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="P12" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>128</v>
-      </c>
-      <c r="R12" s="7" t="s">
-        <v>125</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>129</v>
-      </c>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B15" s="11"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A13" s="11"/>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>152</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="C16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" t="s">
+        <v>154</v>
+      </c>
+      <c r="E16" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>161</v>
+      </c>
+      <c r="M16" t="s">
+        <v>162</v>
+      </c>
+      <c r="N16" t="s">
+        <v>163</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>166</v>
+      </c>
+      <c r="R16" t="s">
+        <v>167</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>168</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>163</v>
+      </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="A14" s="11"/>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="B17" s="11"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="11"/>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B20" s="11"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="11"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="11"/>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B21" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="B7:H7"/>
-    <mergeCell ref="N1:O1"/>
-    <mergeCell ref="P1:Q1"/>
-    <mergeCell ref="R1:S1"/>
-    <mergeCell ref="J1:K1"/>
-    <mergeCell ref="L1:M1"/>
+  <mergeCells count="8">
+    <mergeCell ref="A4:A14"/>
+    <mergeCell ref="C3:I3"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
The cluster weights are now normalized during the training process
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46BAF90F-7A1A-4CE2-B17F-047CEFAB9538}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{493B14B8-2CDA-481A-838F-413BD6B94BFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -242,12 +242,63 @@
         </r>
       </text>
     </comment>
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{D5F8BD09-03BB-4D4F-821A-6D67D15BEEDE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+This trial is called Case 3. Cheat as it cheats into taking the weights from the last epoch of Case 3.d, and train the model from scatch with them.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{2669DDCA-5B47-48AE-91EC-BA0FAB0A2084}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The update rule is the same as case 3c. The difference is that the weights are normalized at each epoch in the following way.
+Let w_(i) be the weight vector at epoch i:
+w_(i+1) = a_(i) * gradient_update(w_(i)) / a_(i+1)
+where a_(i) = sum(w_(i) * cluster_sizes)</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="196">
   <si>
     <t>Training acc</t>
   </si>
@@ -633,9 +684,6 @@
     <t>0.09</t>
   </si>
   <si>
-    <t>Case 3. Cheat</t>
-  </si>
-  <si>
     <t>0.797 +/- 0.0049</t>
   </si>
   <si>
@@ -672,9 +720,6 @@
     <t>0.783 +/- 0.001</t>
   </si>
   <si>
-    <t>0.0748 +/- 0.007</t>
-  </si>
-  <si>
     <t>0.912 +/- 0.001</t>
   </si>
   <si>
@@ -757,6 +802,90 @@
   </si>
   <si>
     <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_160\Run_0</t>
+  </si>
+  <si>
+    <t>0.748 +/- 0.007</t>
+  </si>
+  <si>
+    <t>Case 3d.</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_160\Run_1</t>
+  </si>
+  <si>
+    <t>0.797 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.734 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.805 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.807 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.876 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.063</t>
+  </si>
+  <si>
+    <t>0.066</t>
+  </si>
+  <si>
+    <t>0.071</t>
+  </si>
+  <si>
+    <t>0.073</t>
+  </si>
+  <si>
+    <t>0.068</t>
+  </si>
+  <si>
+    <t>0.069</t>
+  </si>
+  <si>
+    <t>Case 3d Cheat</t>
+  </si>
+  <si>
+    <t>Case 3a. Cheat</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_40\Run_6</t>
+  </si>
+  <si>
+    <t>0.790 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.802 +/- 0.001</t>
+  </si>
+  <si>
+    <t>0.734 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.815 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.795 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.860 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.07</t>
+  </si>
+  <si>
+    <t>0.058</t>
+  </si>
+  <si>
+    <t>0.083</t>
+  </si>
+  <si>
+    <t>0.055</t>
+  </si>
+  <si>
+    <t>0.075</t>
   </si>
 </sst>
 </file>
@@ -864,7 +993,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -887,6 +1016,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1183,10 +1315,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T21"/>
+  <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B25" sqref="A23:B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1240,26 +1372,26 @@
       <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="17" t="s">
+      <c r="K1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="15" t="s">
+      <c r="L1" s="18"/>
+      <c r="M1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16" t="s">
+      <c r="N1" s="16"/>
+      <c r="O1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="15" t="s">
+      <c r="P1" s="17"/>
+      <c r="Q1" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="15"/>
-      <c r="S1" s="16" t="s">
+      <c r="R1" s="16"/>
+      <c r="S1" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="T1" s="16"/>
+      <c r="T1" s="17"/>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="3" t="s">
@@ -1297,17 +1429,17 @@
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
+      <c r="C3" s="16"/>
+      <c r="D3" s="16"/>
+      <c r="E3" s="16"/>
+      <c r="F3" s="16"/>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="15" t="s">
-        <v>151</v>
+      <c r="A4" s="16" t="s">
+        <v>149</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
@@ -1365,7 +1497,7 @@
       </c>
     </row>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="15"/>
+      <c r="A5" s="16"/>
       <c r="B5" s="1" t="s">
         <v>82</v>
       </c>
@@ -1422,7 +1554,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="15"/>
+      <c r="A6" s="16"/>
       <c r="B6" s="8" t="s">
         <v>83</v>
       </c>
@@ -1479,19 +1611,19 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="15"/>
+      <c r="A7" s="16"/>
       <c r="B7" s="9"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
+      <c r="C7" s="16"/>
+      <c r="D7" s="16"/>
+      <c r="E7" s="16"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16"/>
+      <c r="I7" s="16"/>
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="15"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="9" t="s">
         <v>3</v>
       </c>
@@ -1548,7 +1680,7 @@
       </c>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="15"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="9" t="s">
         <v>83</v>
       </c>
@@ -1605,7 +1737,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="15"/>
+      <c r="A10" s="16"/>
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
@@ -1615,7 +1747,7 @@
       <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="15"/>
+      <c r="A11" s="16"/>
       <c r="B11" s="9" t="s">
         <v>112</v>
       </c>
@@ -1626,7 +1758,7 @@
         <v>99</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F11" s="12" t="s">
         <v>100</v>
@@ -1672,30 +1804,30 @@
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="15"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="14" t="s">
-        <v>128</v>
+        <v>183</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D12" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="11" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="F12" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="G12" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="12" t="s">
         <v>131</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="13" t="s">
         <v>132</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>133</v>
       </c>
       <c r="K12" s="7"/>
       <c r="L12" s="7"/>
@@ -1705,7 +1837,7 @@
       <c r="T12" s="7"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="15"/>
+      <c r="A13" s="16"/>
       <c r="B13" s="10" t="s">
         <v>113</v>
       </c>
@@ -1762,42 +1894,42 @@
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="15"/>
+      <c r="A14" s="16"/>
       <c r="B14" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="C14" t="s">
         <v>137</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" s="11" t="s">
         <v>138</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="E14" t="s">
         <v>139</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="G14" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="H14" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="I14" s="13" t="s">
         <v>142</v>
       </c>
-      <c r="H14" s="12" t="s">
+      <c r="K14" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="I14" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>145</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>45</v>
       </c>
       <c r="M14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="N14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="O14" s="7" t="s">
         <v>11</v>
@@ -1806,105 +1938,220 @@
         <v>127</v>
       </c>
       <c r="Q14" t="s">
+        <v>146</v>
+      </c>
+      <c r="R14" t="s">
+        <v>147</v>
+      </c>
+      <c r="S14" s="7" t="s">
         <v>148</v>
-      </c>
-      <c r="R14" t="s">
-        <v>149</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>150</v>
       </c>
       <c r="T14" s="7" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B15" s="11"/>
+      <c r="A15" s="16"/>
+      <c r="B15" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E15" t="s">
+        <v>186</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="H15" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M15" t="s">
+        <v>147</v>
+      </c>
+      <c r="N15" t="s">
+        <v>192</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>179</v>
+      </c>
+      <c r="R15" t="s">
+        <v>195</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A17" s="16" t="s">
+        <v>150</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>151</v>
+      </c>
+      <c r="C17" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" t="s">
         <v>152</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="E17" t="s">
         <v>153</v>
       </c>
-      <c r="C16" t="s">
+      <c r="F17" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K17" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="L17" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M17" t="s">
+        <v>160</v>
+      </c>
+      <c r="N17" t="s">
+        <v>161</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>164</v>
+      </c>
+      <c r="R17" t="s">
+        <v>165</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="T17" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A18" s="16"/>
+      <c r="B18" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D16" t="s">
-        <v>154</v>
-      </c>
-      <c r="E16" t="s">
-        <v>155</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="G16" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="H16" s="12" t="s">
-        <v>158</v>
-      </c>
-      <c r="I16" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="K16" s="7" t="s">
-        <v>160</v>
-      </c>
-      <c r="L16" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="M16" t="s">
-        <v>162</v>
-      </c>
-      <c r="N16" t="s">
-        <v>163</v>
-      </c>
-      <c r="O16" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>166</v>
-      </c>
-      <c r="R16" t="s">
-        <v>167</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>163</v>
+      <c r="C18" t="s">
+        <v>170</v>
+      </c>
+      <c r="D18" t="s">
+        <v>171</v>
+      </c>
+      <c r="E18" t="s">
+        <v>153</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>176</v>
+      </c>
+      <c r="M18" t="s">
+        <v>177</v>
+      </c>
+      <c r="N18" t="s">
+        <v>178</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>179</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>178</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
     </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.35">
-      <c r="B20" s="11"/>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
       <c r="B21" s="11"/>
     </row>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="B22" s="11"/>
+    </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="A4:A14"/>
+  <mergeCells count="9">
+    <mergeCell ref="S1:T1"/>
+    <mergeCell ref="K1:L1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="A17:A18"/>
+    <mergeCell ref="A4:A15"/>
     <mergeCell ref="C3:I3"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
The approah can now optimize for subgroup fairness - can now handle more than one protected attribute
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9377B41E-B47E-4DFF-BD60-625E743D1578}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0255177-9EAF-4733-8D21-68B56E4CFF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
     <author>Gabriel Hayat</author>
   </authors>
   <commentList>
-    <comment ref="C3" authorId="0" shapeId="0" xr:uid="{853C7786-0175-49FB-A01E-8E1EA80AE0B4}">
+    <comment ref="C4" authorId="0" shapeId="0" xr:uid="{853C7786-0175-49FB-A01E-8E1EA80AE0B4}">
       <text>
         <r>
           <rPr>
@@ -63,7 +63,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J5" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
+    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{4256F220-C083-459A-A9ED-B68BB2C9118E}">
       <text>
         <r>
           <rPr>
@@ -88,7 +88,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
+    <comment ref="J7" authorId="0" shapeId="0" xr:uid="{2BCFE6C4-DC80-4788-875E-993B0B22BC6B}">
       <text>
         <r>
           <rPr>
@@ -114,7 +114,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{B1B0EECE-82BA-4961-B120-51E80FE68B69}">
+    <comment ref="C8" authorId="0" shapeId="0" xr:uid="{B1B0EECE-82BA-4961-B120-51E80FE68B69}">
       <text>
         <r>
           <rPr>
@@ -138,7 +138,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{54CBADAE-66FB-43A8-9458-E34F3EB4A4A1}">
+    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{54CBADAE-66FB-43A8-9458-E34F3EB4A4A1}">
       <text>
         <r>
           <rPr>
@@ -164,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J12" authorId="0" shapeId="0" xr:uid="{3F5E49D1-8C77-466D-AB69-2E3A4F4FEB46}">
+    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{3F5E49D1-8C77-466D-AB69-2E3A4F4FEB46}">
       <text>
         <r>
           <rPr>
@@ -190,7 +190,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J13" authorId="0" shapeId="0" xr:uid="{07BB9D53-FAF3-410B-B71D-53A991FB2529}">
+    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{07BB9D53-FAF3-410B-B71D-53A991FB2529}">
       <text>
         <r>
           <rPr>
@@ -216,7 +216,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J14" authorId="0" shapeId="0" xr:uid="{E92869DF-B279-4286-B130-8DBDA1241BD0}">
+    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{E92869DF-B279-4286-B130-8DBDA1241BD0}">
       <text>
         <r>
           <rPr>
@@ -242,7 +242,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J15" authorId="0" shapeId="0" xr:uid="{D5F8BD09-03BB-4D4F-821A-6D67D15BEEDE}">
+    <comment ref="J16" authorId="0" shapeId="0" xr:uid="{D5F8BD09-03BB-4D4F-821A-6D67D15BEEDE}">
       <text>
         <r>
           <rPr>
@@ -266,7 +266,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J18" authorId="0" shapeId="0" xr:uid="{2669DDCA-5B47-48AE-91EC-BA0FAB0A2084}">
+    <comment ref="J19" authorId="0" shapeId="0" xr:uid="{2669DDCA-5B47-48AE-91EC-BA0FAB0A2084}">
       <text>
         <r>
           <rPr>
@@ -293,12 +293,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="N25" authorId="0" shapeId="0" xr:uid="{6437AB48-C207-4578-8AB5-23E9A25B53F8}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Like in the case of group fairnesss, Case_1 repsesents when the model is trained on the bias dataset. Like previously, the test set it is evaluated on is fair, meaning that there are approximately 25% of samples from each subgroup in each class </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N26" authorId="0" shapeId="0" xr:uid="{AAC2A1B6-59E1-47A5-AC9D-5786B9C47EF5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Gabriel Hayat:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+As previously, the weights are dynamically updated and normalised at each epoch, with the update rule being the one described above. </t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="248">
   <si>
     <t>Training acc</t>
   </si>
@@ -886,6 +934,162 @@
   </si>
   <si>
     <t>0.075</t>
+  </si>
+  <si>
+    <t>GROUP FAIRNESS</t>
+  </si>
+  <si>
+    <t>SUBGROUP FAIRNESS</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_1\checkpoints\model_ep_40\Run_2</t>
+  </si>
+  <si>
+    <t>Training acc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test acc. </t>
+  </si>
+  <si>
+    <t>MW</t>
+  </si>
+  <si>
+    <t>FB</t>
+  </si>
+  <si>
+    <t>FW</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>&lt;= 50K</t>
+  </si>
+  <si>
+    <t>&gt;= 50K</t>
+  </si>
+  <si>
+    <t>Female Black (FB)</t>
+  </si>
+  <si>
+    <t>Female White (FW)</t>
+  </si>
+  <si>
+    <t>Male Black (MB)</t>
+  </si>
+  <si>
+    <t>Male White (MW)</t>
+  </si>
+  <si>
+    <t>Case_3d</t>
+  </si>
+  <si>
+    <t>&lt; 50K Max Diff</t>
+  </si>
+  <si>
+    <t>&gt; 50K Max Diff</t>
+  </si>
+  <si>
+    <t>C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\Case_3\checkpoints\model_ep_160\Run_2</t>
+  </si>
+  <si>
+    <t>0.760 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.78 +/- 0</t>
+  </si>
+  <si>
+    <t>0.072</t>
+  </si>
+  <si>
+    <t>0.067</t>
+  </si>
+  <si>
+    <t>0.099</t>
+  </si>
+  <si>
+    <t>0.801 +/- 0.0009</t>
+  </si>
+  <si>
+    <t>0.929 +/- 0.009</t>
+  </si>
+  <si>
+    <t>0.9135+/- 0.005</t>
+  </si>
+  <si>
+    <t>0.775 +/- 0.014</t>
+  </si>
+  <si>
+    <t>0.623 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.503 +/- 0.025</t>
+  </si>
+  <si>
+    <t>0.688 +/- 0.009</t>
+  </si>
+  <si>
+    <t>0.742 +/- 0.008</t>
+  </si>
+  <si>
+    <t>0.871 +/- 0.008</t>
+  </si>
+  <si>
+    <t>0.31</t>
+  </si>
+  <si>
+    <t>0.416</t>
+  </si>
+  <si>
+    <t>0.294</t>
+  </si>
+  <si>
+    <t>0.341</t>
+  </si>
+  <si>
+    <t>0.360</t>
+  </si>
+  <si>
+    <t>0.327</t>
+  </si>
+  <si>
+    <t>0.393</t>
+  </si>
+  <si>
+    <t>0.332</t>
+  </si>
+  <si>
+    <t>0.798 +/- 0.0008</t>
+  </si>
+  <si>
+    <t>0.8008 +/- 0.0009</t>
+  </si>
+  <si>
+    <t>0.773  +/- 0.005</t>
+  </si>
+  <si>
+    <t>0.797 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.759 +/- 0.003</t>
+  </si>
+  <si>
+    <t>0.731 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.880 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.868 +/- 0.002</t>
+  </si>
+  <si>
+    <t>0.812 +/- 0.004</t>
+  </si>
+  <si>
+    <t>0.0068</t>
+  </si>
+  <si>
+    <t>0.103</t>
   </si>
 </sst>
 </file>
@@ -928,7 +1132,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -955,6 +1159,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -986,14 +1208,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1022,20 +1247,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="8">
     <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="5" builtinId="35"/>
     <cellStyle name="40% - Accent3" xfId="4" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="6" builtinId="43"/>
     <cellStyle name="40% - Accent5" xfId="3" builtinId="47"/>
+    <cellStyle name="40% - Accent6" xfId="7" builtinId="51"/>
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -1315,10 +1562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T22"/>
+  <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" topLeftCell="S10" workbookViewId="0">
+      <selection activeCell="X26" sqref="X26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1333,825 +1580,1144 @@
     <col min="8" max="8" width="15.453125" customWidth="1"/>
     <col min="9" max="9" width="16.453125" customWidth="1"/>
     <col min="10" max="10" width="18.54296875" customWidth="1"/>
-    <col min="11" max="11" width="13.26953125" customWidth="1"/>
-    <col min="12" max="13" width="12.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="13" width="14.36328125" customWidth="1"/>
     <col min="14" max="14" width="13.1796875" customWidth="1"/>
     <col min="15" max="15" width="12.7265625" customWidth="1"/>
     <col min="16" max="16" width="12.453125" customWidth="1"/>
     <col min="17" max="17" width="12.54296875" customWidth="1"/>
     <col min="18" max="18" width="12.7265625" customWidth="1"/>
-    <col min="19" max="19" width="12.90625" customWidth="1"/>
-    <col min="20" max="20" width="12" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="13" customWidth="1"/>
+    <col min="21" max="23" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" t="s">
-        <v>1</v>
-      </c>
-      <c r="K1" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" s="17"/>
-      <c r="M1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="N1" s="18"/>
-      <c r="O1" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="R1" s="18"/>
-      <c r="S1" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="T1" s="16"/>
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A1" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="25"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="25"/>
+      <c r="P1" s="25"/>
+      <c r="Q1" s="25"/>
+      <c r="R1" s="25"/>
+      <c r="S1" s="25"/>
+      <c r="T1" s="25"/>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K2" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="27"/>
+      <c r="M2" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="N2" s="25"/>
+      <c r="O2" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" s="25"/>
+      <c r="S2" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="T2" s="26"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="N2" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q3" t="s">
         <v>17</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R3" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T3" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-    </row>
-    <row r="4" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="18" t="s">
-        <v>149</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="M4" t="s">
-        <v>31</v>
-      </c>
-      <c r="N4" t="s">
-        <v>32</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>29</v>
-      </c>
-      <c r="R4" t="s">
-        <v>30</v>
-      </c>
-      <c r="S4" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="T4" s="6" t="s">
-        <v>13</v>
-      </c>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
     </row>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="18"/>
+      <c r="A5" s="25" t="s">
+        <v>149</v>
+      </c>
       <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R5" t="s">
+        <v>30</v>
+      </c>
+      <c r="S5" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A6" s="25"/>
+      <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>62</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E6" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F6" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="L5" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M6" t="s">
         <v>41</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N6" t="s">
         <v>47</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O6" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="P5" s="6" t="s">
+      <c r="P6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="Q6" t="s">
         <v>43</v>
       </c>
-      <c r="R5" t="s">
+      <c r="R6" t="s">
         <v>44</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T6" s="6" t="s">
         <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A6" s="18"/>
-      <c r="B6" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="C6" t="s">
-        <v>63</v>
-      </c>
-      <c r="D6" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="K6" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="L6" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M6" t="s">
-        <v>56</v>
-      </c>
-      <c r="N6" t="s">
-        <v>57</v>
-      </c>
-      <c r="O6" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="P6" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>56</v>
-      </c>
-      <c r="R6" t="s">
-        <v>59</v>
-      </c>
-      <c r="S6" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="T6" s="7" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="18"/>
-      <c r="B7" s="9"/>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="9"/>
+      <c r="A7" s="25"/>
+      <c r="B7" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="C7" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="K7" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L7" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M7" t="s">
+        <v>56</v>
+      </c>
+      <c r="N7" t="s">
+        <v>57</v>
+      </c>
+      <c r="O7" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="P7" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7" t="s">
+        <v>59</v>
+      </c>
+      <c r="S7" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="T7" s="7" t="s">
+        <v>59</v>
+      </c>
     </row>
-    <row r="8" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="18"/>
-      <c r="B8" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-      <c r="E8" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="L8" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="M8" t="s">
-        <v>74</v>
-      </c>
-      <c r="N8" t="s">
-        <v>75</v>
-      </c>
-      <c r="O8" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="P8" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>78</v>
-      </c>
-      <c r="R8" t="s">
-        <v>79</v>
-      </c>
-      <c r="S8" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>81</v>
-      </c>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+      <c r="A8" s="25"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="25"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
+      <c r="I8" s="25"/>
+      <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="18"/>
+      <c r="A9" s="25"/>
       <c r="B9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" t="s">
+        <v>67</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="M9" t="s">
+        <v>74</v>
+      </c>
+      <c r="N9" t="s">
+        <v>75</v>
+      </c>
+      <c r="O9" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="P9" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>78</v>
+      </c>
+      <c r="R9" t="s">
+        <v>79</v>
+      </c>
+      <c r="S9" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="T9" s="6" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A10" s="25"/>
+      <c r="B10" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>85</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>86</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" t="s">
         <v>30</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" t="s">
         <v>93</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O10" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="P9" s="6" t="s">
+      <c r="P10" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q10" t="s">
         <v>96</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R10" t="s">
         <v>92</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="S10" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="T10" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A10" s="18"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="18"/>
-      <c r="B11" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="E11" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>100</v>
-      </c>
-      <c r="G11" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="H11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>103</v>
-      </c>
-      <c r="K11" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="M11" t="s">
-        <v>104</v>
-      </c>
-      <c r="N11" t="s">
-        <v>105</v>
-      </c>
-      <c r="O11" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="P11" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>108</v>
-      </c>
-      <c r="R11" t="s">
-        <v>109</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="T11" s="7" t="s">
-        <v>111</v>
-      </c>
+      <c r="A11" s="25"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11"/>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="18"/>
-      <c r="B12" s="14" t="s">
-        <v>183</v>
+      <c r="A12" s="25"/>
+      <c r="B12" s="9" t="s">
+        <v>112</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>135</v>
+        <v>98</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>129</v>
+        <v>100</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>130</v>
+        <v>101</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>131</v>
+        <v>102</v>
       </c>
       <c r="I12" s="13" t="s">
-        <v>132</v>
-      </c>
-      <c r="K12" s="7"/>
-      <c r="L12" s="7"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="7"/>
-      <c r="S12" s="7"/>
-      <c r="T12" s="7"/>
+        <v>103</v>
+      </c>
+      <c r="K12" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="L12" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="M12" t="s">
+        <v>104</v>
+      </c>
+      <c r="N12" t="s">
+        <v>105</v>
+      </c>
+      <c r="O12" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="P12" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>108</v>
+      </c>
+      <c r="R12" t="s">
+        <v>109</v>
+      </c>
+      <c r="S12" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="T12" s="7" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="18"/>
-      <c r="B13" s="10" t="s">
-        <v>113</v>
+      <c r="A13" s="25"/>
+      <c r="B13" s="14" t="s">
+        <v>183</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>114</v>
+        <v>135</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>115</v>
+        <v>133</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>117</v>
+        <v>129</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>118</v>
+        <v>130</v>
       </c>
       <c r="H13" s="12" t="s">
-        <v>119</v>
+        <v>131</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>120</v>
-      </c>
-      <c r="K13" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="M13" t="s">
-        <v>123</v>
-      </c>
-      <c r="N13" t="s">
-        <v>104</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="P13" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>125</v>
-      </c>
-      <c r="R13" t="s">
-        <v>126</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>123</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>127</v>
-      </c>
+        <v>132</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="18"/>
-      <c r="B14" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="C14" t="s">
-        <v>137</v>
+      <c r="A14" s="25"/>
+      <c r="B14" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>114</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="E14" t="s">
-        <v>139</v>
+        <v>115</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>116</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>168</v>
+        <v>117</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="H14" s="12" t="s">
-        <v>141</v>
+        <v>119</v>
       </c>
       <c r="I14" s="13" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="K14" s="7" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="L14" s="7" t="s">
-        <v>45</v>
+        <v>122</v>
       </c>
       <c r="M14" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="N14" t="s">
-        <v>145</v>
+        <v>104</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="P14" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>125</v>
+      </c>
+      <c r="R14" t="s">
+        <v>126</v>
+      </c>
+      <c r="S14" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="T14" s="7" t="s">
         <v>127</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>146</v>
-      </c>
-      <c r="R14" t="s">
-        <v>147</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>148</v>
-      </c>
-      <c r="T14" s="7" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="18"/>
-      <c r="B15" s="15" t="s">
-        <v>182</v>
+      <c r="A15" s="25"/>
+      <c r="B15" s="14" t="s">
+        <v>136</v>
       </c>
       <c r="C15" t="s">
-        <v>184</v>
+        <v>137</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>185</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
-        <v>186</v>
+        <v>139</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>187</v>
+        <v>168</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>188</v>
+        <v>140</v>
       </c>
       <c r="H15" s="12" t="s">
-        <v>189</v>
+        <v>141</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>190</v>
+        <v>142</v>
       </c>
       <c r="K15" s="7" t="s">
-        <v>191</v>
+        <v>143</v>
       </c>
       <c r="L15" s="7" t="s">
-        <v>181</v>
+        <v>45</v>
       </c>
       <c r="M15" t="s">
+        <v>144</v>
+      </c>
+      <c r="N15" t="s">
+        <v>145</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>146</v>
+      </c>
+      <c r="R15" t="s">
         <v>147</v>
       </c>
-      <c r="N15" t="s">
-        <v>192</v>
-      </c>
-      <c r="O15" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="P15" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>179</v>
-      </c>
-      <c r="R15" t="s">
-        <v>195</v>
-      </c>
       <c r="S15" s="7" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="T15" s="7" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B16" s="11"/>
+      <c r="A16" s="25"/>
+      <c r="B16" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" t="s">
+        <v>184</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>185</v>
+      </c>
+      <c r="E16" t="s">
+        <v>186</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="K16" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>181</v>
+      </c>
+      <c r="M16" t="s">
+        <v>147</v>
+      </c>
+      <c r="N16" t="s">
+        <v>192</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>179</v>
+      </c>
+      <c r="R16" t="s">
+        <v>195</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>181</v>
+      </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A17" s="18" t="s">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A18" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B18" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C18" t="s">
         <v>167</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D18" t="s">
         <v>152</v>
-      </c>
-      <c r="E17" t="s">
-        <v>153</v>
-      </c>
-      <c r="F17" s="12" t="s">
-        <v>154</v>
-      </c>
-      <c r="G17" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="H17" s="12" t="s">
-        <v>156</v>
-      </c>
-      <c r="I17" s="13" t="s">
-        <v>157</v>
-      </c>
-      <c r="K17" s="7" t="s">
-        <v>158</v>
-      </c>
-      <c r="L17" s="7" t="s">
-        <v>159</v>
-      </c>
-      <c r="M17" t="s">
-        <v>160</v>
-      </c>
-      <c r="N17" t="s">
-        <v>161</v>
-      </c>
-      <c r="O17" s="7" t="s">
-        <v>162</v>
-      </c>
-      <c r="P17" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>164</v>
-      </c>
-      <c r="R17" t="s">
-        <v>165</v>
-      </c>
-      <c r="S17" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A18" s="18"/>
-      <c r="B18" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C18" t="s">
-        <v>170</v>
-      </c>
-      <c r="D18" t="s">
-        <v>171</v>
       </c>
       <c r="E18" t="s">
         <v>153</v>
       </c>
       <c r="F18" s="12" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="K18" s="7" t="s">
+        <v>158</v>
+      </c>
+      <c r="L18" s="7" t="s">
+        <v>159</v>
+      </c>
+      <c r="M18" t="s">
+        <v>160</v>
+      </c>
+      <c r="N18" t="s">
+        <v>161</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>164</v>
+      </c>
+      <c r="R18" t="s">
+        <v>165</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A19" s="25"/>
+      <c r="B19" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C19" t="s">
+        <v>170</v>
+      </c>
+      <c r="D19" t="s">
+        <v>171</v>
+      </c>
+      <c r="E19" t="s">
+        <v>153</v>
+      </c>
+      <c r="F19" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="G18" s="13" t="s">
+      <c r="G19" s="13" t="s">
         <v>173</v>
       </c>
-      <c r="H18" s="12" t="s">
+      <c r="H19" s="12" t="s">
         <v>174</v>
       </c>
-      <c r="I18" s="13" t="s">
+      <c r="I19" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="K18" s="7" t="s">
+      <c r="K19" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="L18" s="7" t="s">
+      <c r="L19" s="7" t="s">
         <v>176</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M19" t="s">
         <v>177</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N19" t="s">
         <v>178</v>
       </c>
-      <c r="O18" s="7" t="s">
+      <c r="O19" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="P18" s="7" t="s">
+      <c r="P19" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="Q18" s="7" t="s">
+      <c r="Q19" s="7" t="s">
         <v>180</v>
       </c>
-      <c r="R18" s="7" t="s">
+      <c r="R19" s="7" t="s">
         <v>181</v>
       </c>
-      <c r="S18" s="7" t="s">
+      <c r="S19" s="7" t="s">
         <v>177</v>
       </c>
-      <c r="T18" s="7" t="s">
+      <c r="T19" s="7" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B21" s="11"/>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A21" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
+      <c r="G21" s="25"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="25"/>
+      <c r="J21" s="25"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="25"/>
+      <c r="M21" s="25"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="25"/>
+      <c r="P21" s="25"/>
+      <c r="Q21" s="25"/>
+      <c r="R21" s="25"/>
+      <c r="S21" s="25"/>
+      <c r="T21" s="25"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="B22" s="11"/>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A22" s="16"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>208</v>
+      </c>
+      <c r="F22" s="21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="H22" s="16"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="16"/>
+      <c r="K22" s="16"/>
+      <c r="L22" s="16"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="P22" s="25"/>
+      <c r="Q22" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="R22" s="25"/>
+      <c r="S22" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="T22" s="25"/>
+      <c r="U22" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="V22" s="25"/>
+      <c r="W22" s="25" t="s">
+        <v>10</v>
+      </c>
+      <c r="X22" s="25"/>
+    </row>
+    <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="11"/>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>199</v>
+      </c>
+      <c r="E23" t="s">
+        <v>200</v>
+      </c>
+      <c r="F23" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="G23" s="25"/>
+      <c r="H23" s="25"/>
+      <c r="I23" s="25"/>
+      <c r="J23" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="K23" s="25"/>
+      <c r="L23" s="25"/>
+      <c r="M23" s="25"/>
+      <c r="O23" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="P23" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>212</v>
+      </c>
+      <c r="R23" t="s">
+        <v>213</v>
+      </c>
+      <c r="S23" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="T23" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="U23" t="s">
+        <v>17</v>
+      </c>
+      <c r="V23" t="s">
+        <v>213</v>
+      </c>
+      <c r="W23" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="X23" s="5" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B24" s="11"/>
+      <c r="F24" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="G24" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="H24" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="J24" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="K24" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="L24" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>149</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" t="s">
+        <v>215</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>221</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>225</v>
+      </c>
+      <c r="K25" s="20" t="s">
+        <v>226</v>
+      </c>
+      <c r="L25" s="22" t="s">
+        <v>227</v>
+      </c>
+      <c r="M25" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="O25" s="24" t="s">
+        <v>229</v>
+      </c>
+      <c r="P25" s="24" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>231</v>
+      </c>
+      <c r="R25" t="s">
+        <v>232</v>
+      </c>
+      <c r="S25" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="T25" s="24" t="s">
+        <v>233</v>
+      </c>
+      <c r="U25" t="s">
+        <v>234</v>
+      </c>
+      <c r="V25" t="s">
+        <v>235</v>
+      </c>
+      <c r="W25" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="X25" s="24" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="C26" t="s">
+        <v>214</v>
+      </c>
+      <c r="D26" t="s">
+        <v>237</v>
+      </c>
+      <c r="E26" t="s">
+        <v>238</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>239</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>240</v>
+      </c>
+      <c r="H26" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="J26" s="18" t="s">
+        <v>243</v>
+      </c>
+      <c r="K26" s="20" t="s">
+        <v>244</v>
+      </c>
+      <c r="L26" s="22" t="s">
+        <v>245</v>
+      </c>
+      <c r="M26" s="4" t="s">
+        <v>216</v>
+      </c>
+      <c r="O26" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>246</v>
+      </c>
+      <c r="R26" t="s">
+        <v>219</v>
+      </c>
+      <c r="S26" s="24" t="s">
+        <v>192</v>
+      </c>
+      <c r="T26" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="U26" t="s">
+        <v>218</v>
+      </c>
+      <c r="V26" t="s">
+        <v>219</v>
+      </c>
+      <c r="W26" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="X26" s="24" t="s">
+        <v>219</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="S1:T1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="A17:A18"/>
-    <mergeCell ref="A4:A15"/>
-    <mergeCell ref="C3:I3"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="O1:P1"/>
-    <mergeCell ref="Q1:R1"/>
+  <mergeCells count="18">
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="A21:T21"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="O22:P22"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A5:A16"/>
+    <mergeCell ref="C4:I4"/>
+    <mergeCell ref="C8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactoring code + added comments
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0255177-9EAF-4733-8D21-68B56E4CFF02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D1DC89-B219-404C-9896-4A299BCD8D5B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="14400" windowHeight="7810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1266,10 +1266,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
@@ -1564,8 +1564,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S10" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1594,28 +1594,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="26" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25"/>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25"/>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25"/>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25"/>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25"/>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25"/>
-      <c r="T1" s="25"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="I1" s="26"/>
+      <c r="J1" s="26"/>
+      <c r="K1" s="26"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="26"/>
+      <c r="N1" s="26"/>
+      <c r="O1" s="26"/>
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26"/>
+      <c r="R1" s="26"/>
+      <c r="S1" s="26"/>
+      <c r="T1" s="26"/>
     </row>
     <row r="2" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
@@ -1649,22 +1649,22 @@
         <v>6</v>
       </c>
       <c r="L2" s="27"/>
-      <c r="M2" s="25" t="s">
+      <c r="M2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="25"/>
-      <c r="O2" s="26" t="s">
+      <c r="N2" s="26"/>
+      <c r="O2" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="25" t="s">
+      <c r="P2" s="25"/>
+      <c r="Q2" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="R2" s="25"/>
-      <c r="S2" s="26" t="s">
+      <c r="R2" s="26"/>
+      <c r="S2" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="T2" s="26"/>
+      <c r="T2" s="25"/>
     </row>
     <row r="3" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="3" t="s">
@@ -1702,16 +1702,16 @@
       </c>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="26"/>
+      <c r="H4" s="26"/>
+      <c r="I4" s="26"/>
     </row>
     <row r="5" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="26" t="s">
         <v>149</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1770,7 +1770,7 @@
       </c>
     </row>
     <row r="6" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="1" t="s">
         <v>82</v>
       </c>
@@ -1827,7 +1827,7 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="8" t="s">
         <v>83</v>
       </c>
@@ -1884,19 +1884,19 @@
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="9"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="25"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
+      <c r="E8" s="26"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="26"/>
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="9" t="s">
         <v>3</v>
       </c>
@@ -1953,7 +1953,7 @@
       </c>
     </row>
     <row r="10" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="9" t="s">
         <v>83</v>
       </c>
@@ -2010,7 +2010,7 @@
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
@@ -2020,7 +2020,7 @@
       <c r="I11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="9" t="s">
         <v>112</v>
       </c>
@@ -2077,7 +2077,7 @@
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
+      <c r="A13" s="26"/>
       <c r="B13" s="14" t="s">
         <v>183</v>
       </c>
@@ -2110,7 +2110,7 @@
       <c r="T13" s="7"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A14" s="25"/>
+      <c r="A14" s="26"/>
       <c r="B14" s="10" t="s">
         <v>113</v>
       </c>
@@ -2167,7 +2167,7 @@
       </c>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A15" s="25"/>
+      <c r="A15" s="26"/>
       <c r="B15" s="14" t="s">
         <v>136</v>
       </c>
@@ -2224,7 +2224,7 @@
       </c>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.35">
-      <c r="A16" s="25"/>
+      <c r="A16" s="26"/>
       <c r="B16" s="15" t="s">
         <v>182</v>
       </c>
@@ -2284,7 +2284,7 @@
       <c r="B17" s="11"/>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A18" s="25" t="s">
+      <c r="A18" s="26" t="s">
         <v>150</v>
       </c>
       <c r="B18" s="14" t="s">
@@ -2343,7 +2343,7 @@
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A19" s="25"/>
+      <c r="A19" s="26"/>
       <c r="B19" s="15" t="s">
         <v>169</v>
       </c>
@@ -2409,28 +2409,28 @@
       <c r="I20" s="11"/>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.35">
-      <c r="A21" s="25" t="s">
+      <c r="A21" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="B21" s="25"/>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
-      <c r="L21" s="25"/>
-      <c r="M21" s="25"/>
-      <c r="N21" s="25"/>
-      <c r="O21" s="25"/>
-      <c r="P21" s="25"/>
-      <c r="Q21" s="25"/>
-      <c r="R21" s="25"/>
-      <c r="S21" s="25"/>
-      <c r="T21" s="25"/>
+      <c r="B21" s="26"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="26"/>
+      <c r="J21" s="26"/>
+      <c r="K21" s="26"/>
+      <c r="L21" s="26"/>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A22" s="16"/>
@@ -2457,26 +2457,26 @@
       <c r="N22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="O22" s="25" t="s">
+      <c r="O22" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="P22" s="25"/>
-      <c r="Q22" s="25" t="s">
+      <c r="P22" s="26"/>
+      <c r="Q22" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="R22" s="25"/>
-      <c r="S22" s="25" t="s">
+      <c r="R22" s="26"/>
+      <c r="S22" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="T22" s="25"/>
-      <c r="U22" s="25" t="s">
+      <c r="T22" s="26"/>
+      <c r="U22" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="V22" s="25"/>
-      <c r="W22" s="25" t="s">
+      <c r="V22" s="26"/>
+      <c r="W22" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="X22" s="25"/>
+      <c r="X22" s="26"/>
     </row>
     <row r="23" spans="1:24" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B23" s="11"/>
@@ -2489,18 +2489,18 @@
       <c r="E23" t="s">
         <v>200</v>
       </c>
-      <c r="F23" s="25" t="s">
+      <c r="F23" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="25"/>
-      <c r="J23" s="25" t="s">
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="26"/>
+      <c r="J23" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="K23" s="25"/>
-      <c r="L23" s="25"/>
-      <c r="M23" s="25"/>
+      <c r="K23" s="26"/>
+      <c r="L23" s="26"/>
+      <c r="M23" s="26"/>
       <c r="O23" s="5" t="s">
         <v>212</v>
       </c>
@@ -2700,11 +2700,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="U22:V22"/>
-    <mergeCell ref="W22:X22"/>
-    <mergeCell ref="A21:T21"/>
     <mergeCell ref="A1:T1"/>
     <mergeCell ref="F23:I23"/>
     <mergeCell ref="J23:M23"/>
@@ -2718,6 +2713,11 @@
     <mergeCell ref="A5:A16"/>
     <mergeCell ref="C4:I4"/>
     <mergeCell ref="C8:I8"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="A21:T21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>

<commit_message>
Implementation of sample weight updates + documentation added + command parameters added + Code refactoring
</commit_message>
<xml_diff>
--- a/Logistic_Regression/results.xlsx
+++ b/Logistic_Regression/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabriel Hayat\Documents\ETHZ\MsCS\Thesis\Code\Logistic_Regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B1BF8A-8271-4D40-BA4B-305D47664D73}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B61DD1-E667-4F35-81EA-0A5F80E28EAD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -948,9 +948,6 @@
     <t>0.075</t>
   </si>
   <si>
-    <t>GROUP FAIRNESS</t>
-  </si>
-  <si>
     <t>SUBGROUP FAIRNESS</t>
   </si>
   <si>
@@ -1351,6 +1348,9 @@
   </si>
   <si>
     <t>0.269</t>
+  </si>
+  <si>
+    <t>SPREADSHEET IS NO LONGER UP TO DATE, RESULTS FROM NEW EXPERIMENTS ARE REPORTED ON: https://docs.google.com/spreadsheets/d/1ldy0gzoyLDWxHnxsZ5bwZIpUmT3pRPwAWHoosfFtXWI/edit#gid=1745112050</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1479,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1530,13 +1530,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1544,6 +1542,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="8">
@@ -1832,10 +1833,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:Y59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1864,32 +1865,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B1" s="27" t="s">
-        <v>184</v>
-      </c>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
+      <c r="B1" s="28" t="s">
+        <v>318</v>
+      </c>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="28"/>
+      <c r="P1" s="28"/>
+      <c r="Q1" s="28"/>
+      <c r="R1" s="28"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
     </row>
     <row r="2" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="29" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>4</v>
@@ -1918,26 +1919,26 @@
       <c r="K2" t="s">
         <v>1</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="M2" s="28"/>
-      <c r="N2" s="27" t="s">
+      <c r="M2" s="31"/>
+      <c r="N2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="O2" s="27"/>
-      <c r="P2" s="26" t="s">
+      <c r="O2" s="28"/>
+      <c r="P2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="27" t="s">
+      <c r="Q2" s="27"/>
+      <c r="R2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="S2" s="27"/>
-      <c r="T2" s="26" t="s">
+      <c r="S2" s="28"/>
+      <c r="T2" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="U2" s="26"/>
+      <c r="U2" s="27"/>
     </row>
     <row r="3" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="29"/>
@@ -1977,24 +1978,24 @@
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" s="29"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="27"/>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-      <c r="I4" s="27"/>
-      <c r="J4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
     </row>
     <row r="5" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="29"/>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="28" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -2047,12 +2048,12 @@
     </row>
     <row r="6" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="29"/>
-      <c r="B6" s="27"/>
+      <c r="B6" s="28"/>
       <c r="C6" s="1" t="s">
         <v>78</v>
       </c>
       <c r="D6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E6" t="s">
         <v>32</v>
@@ -2105,12 +2106,12 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" s="29"/>
-      <c r="B7" s="27"/>
+      <c r="B7" s="28"/>
       <c r="C7" s="8" t="s">
         <v>79</v>
       </c>
       <c r="D7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E7" t="s">
         <v>61</v>
@@ -2163,25 +2164,25 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" s="29"/>
-      <c r="B8" s="27"/>
+      <c r="B8" s="28"/>
       <c r="C8" s="9"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
       <c r="K8" s="9"/>
     </row>
     <row r="9" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="29"/>
-      <c r="B9" s="27"/>
+      <c r="B9" s="28"/>
       <c r="C9" s="9" t="s">
         <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="E9" t="s">
         <v>62</v>
@@ -2234,12 +2235,12 @@
     </row>
     <row r="10" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A10" s="29"/>
-      <c r="B10" s="27"/>
+      <c r="B10" s="28"/>
       <c r="C10" s="9" t="s">
         <v>79</v>
       </c>
       <c r="D10" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E10" t="s">
         <v>80</v>
@@ -2292,7 +2293,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" s="29"/>
-      <c r="B11" s="27"/>
+      <c r="B11" s="28"/>
       <c r="D11" s="11"/>
       <c r="E11" s="11"/>
       <c r="F11" s="11"/>
@@ -2303,12 +2304,12 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" s="29"/>
-      <c r="B12" s="27"/>
+      <c r="B12" s="28"/>
       <c r="C12" s="9" t="s">
         <v>106</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>93</v>
@@ -2361,12 +2362,12 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" s="29"/>
-      <c r="B13" s="27"/>
+      <c r="B13" s="28"/>
       <c r="C13" s="14" t="s">
         <v>172</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>126</v>
@@ -2395,12 +2396,12 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" s="29"/>
-      <c r="B14" s="27"/>
+      <c r="B14" s="28"/>
       <c r="C14" s="10" t="s">
         <v>107</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E14" s="11" t="s">
         <v>108</v>
@@ -2453,12 +2454,12 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" s="29"/>
-      <c r="B15" s="27"/>
+      <c r="B15" s="28"/>
       <c r="C15" s="14" t="s">
         <v>128</v>
       </c>
       <c r="D15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E15" s="11" t="s">
         <v>129</v>
@@ -2511,12 +2512,12 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" s="29"/>
-      <c r="B16" s="27"/>
+      <c r="B16" s="28"/>
       <c r="C16" s="15" t="s">
         <v>171</v>
       </c>
       <c r="D16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="E16" s="11" t="s">
         <v>173</v>
@@ -2573,14 +2574,14 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" s="29"/>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="28" t="s">
         <v>141</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>142</v>
       </c>
       <c r="D18" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="E18" t="s">
         <v>143</v>
@@ -2633,12 +2634,12 @@
     </row>
     <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" s="29"/>
-      <c r="B19" s="27"/>
+      <c r="B19" s="28"/>
       <c r="C19" s="15" t="s">
         <v>159</v>
       </c>
       <c r="D19" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E19" t="s">
         <v>160</v>
@@ -2701,28 +2702,28 @@
     </row>
     <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" s="29"/>
-      <c r="B21" s="27" t="s">
-        <v>185</v>
-      </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="27"/>
-      <c r="T21" s="27"/>
-      <c r="U21" s="27"/>
+      <c r="B21" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+      <c r="K21" s="28"/>
+      <c r="L21" s="28"/>
+      <c r="M21" s="28"/>
+      <c r="N21" s="28"/>
+      <c r="O21" s="28"/>
+      <c r="P21" s="28"/>
+      <c r="Q21" s="28"/>
+      <c r="R21" s="28"/>
+      <c r="S21" s="28"/>
+      <c r="T21" s="28"/>
+      <c r="U21" s="28"/>
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" s="29"/>
@@ -2730,16 +2731,16 @@
       <c r="C22" s="16"/>
       <c r="D22" s="16"/>
       <c r="E22" s="17" t="s">
+        <v>193</v>
+      </c>
+      <c r="F22" s="19" t="s">
         <v>194</v>
       </c>
-      <c r="F22" s="19" t="s">
+      <c r="G22" s="21" t="s">
         <v>195</v>
       </c>
-      <c r="G22" s="21" t="s">
+      <c r="H22" s="23" t="s">
         <v>196</v>
-      </c>
-      <c r="H22" s="23" t="s">
-        <v>197</v>
       </c>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
@@ -2750,26 +2751,26 @@
       <c r="O22" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="P22" s="27" t="s">
+      <c r="P22" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27" t="s">
+      <c r="Q22" s="28"/>
+      <c r="R22" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27" t="s">
+      <c r="S22" s="28"/>
+      <c r="T22" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27" t="s">
+      <c r="U22" s="28"/>
+      <c r="V22" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27" t="s">
+      <c r="W22" s="28"/>
+      <c r="X22" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="Y22" s="27"/>
+      <c r="Y22" s="28"/>
     </row>
     <row r="23" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="29"/>
@@ -2778,80 +2779,80 @@
         <v>2</v>
       </c>
       <c r="E23" t="s">
+        <v>185</v>
+      </c>
+      <c r="F23" t="s">
         <v>186</v>
       </c>
-      <c r="F23" t="s">
-        <v>187</v>
-      </c>
-      <c r="G23" s="27" t="s">
+      <c r="G23" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27" t="s">
-        <v>193</v>
-      </c>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
       <c r="P23" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q23" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="Q23" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="R23" t="s">
+        <v>198</v>
+      </c>
+      <c r="S23" t="s">
         <v>199</v>
       </c>
-      <c r="S23" t="s">
-        <v>200</v>
-      </c>
       <c r="T23" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="U23" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="U23" s="5" t="s">
-        <v>200</v>
       </c>
       <c r="V23" t="s">
         <v>17</v>
       </c>
       <c r="W23" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="X23" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y23" s="5" t="s">
         <v>199</v>
-      </c>
-      <c r="Y23" s="5" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" s="29"/>
       <c r="C24" s="11"/>
       <c r="G24" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H24" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="H24" s="20" t="s">
+      <c r="I24" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="I24" s="22" t="s">
-        <v>191</v>
-      </c>
       <c r="J24" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="K24" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="K24" s="18" t="s">
+      <c r="L24" s="20" t="s">
         <v>189</v>
       </c>
-      <c r="L24" s="20" t="s">
+      <c r="M24" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="M24" s="22" t="s">
-        <v>191</v>
-      </c>
       <c r="N24" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.35">
@@ -2863,67 +2864,67 @@
         <v>3</v>
       </c>
       <c r="D25" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="E25" t="s">
+        <v>205</v>
+      </c>
+      <c r="F25" t="s">
+        <v>200</v>
+      </c>
+      <c r="G25" s="18" t="s">
         <v>206</v>
       </c>
-      <c r="F25" t="s">
-        <v>201</v>
-      </c>
-      <c r="G25" s="18" t="s">
+      <c r="H25" s="20" t="s">
         <v>207</v>
       </c>
-      <c r="H25" s="20" t="s">
+      <c r="I25" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="J25" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="J25" s="4" t="s">
+      <c r="K25" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="K25" s="18" t="s">
+      <c r="L25" s="20" t="s">
         <v>211</v>
       </c>
-      <c r="L25" s="20" t="s">
+      <c r="M25" s="22" t="s">
         <v>212</v>
       </c>
-      <c r="M25" s="22" t="s">
+      <c r="N25" s="4" t="s">
         <v>213</v>
       </c>
-      <c r="N25" s="4" t="s">
+      <c r="P25" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="P25" s="24" t="s">
+      <c r="Q25" s="24" t="s">
         <v>215</v>
       </c>
-      <c r="Q25" s="24" t="s">
+      <c r="R25" t="s">
         <v>216</v>
       </c>
-      <c r="R25" t="s">
+      <c r="S25" t="s">
         <v>217</v>
-      </c>
-      <c r="S25" t="s">
-        <v>218</v>
       </c>
       <c r="T25" s="24" t="s">
         <v>68</v>
       </c>
       <c r="U25" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="V25" t="s">
         <v>219</v>
       </c>
-      <c r="V25" t="s">
+      <c r="W25" t="s">
         <v>220</v>
-      </c>
-      <c r="W25" t="s">
-        <v>221</v>
       </c>
       <c r="X25" s="24" t="s">
         <v>68</v>
       </c>
       <c r="Y25" s="24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.35">
@@ -2932,190 +2933,190 @@
         <v>141</v>
       </c>
       <c r="C26" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D26" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E26" t="s">
+        <v>222</v>
+      </c>
+      <c r="F26" t="s">
         <v>223</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" s="18" t="s">
         <v>224</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="H26" s="20" t="s">
         <v>225</v>
       </c>
-      <c r="H26" s="20" t="s">
+      <c r="I26" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="J26" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="J26" s="4" t="s">
+      <c r="K26" s="18" t="s">
         <v>228</v>
       </c>
-      <c r="K26" s="18" t="s">
+      <c r="L26" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="L26" s="20" t="s">
+      <c r="M26" s="22" t="s">
         <v>230</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="N26" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="P26" s="24" t="s">
+        <v>202</v>
+      </c>
+      <c r="Q26" s="24" t="s">
+        <v>204</v>
+      </c>
+      <c r="R26" t="s">
         <v>231</v>
       </c>
-      <c r="N26" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="P26" s="24" t="s">
-        <v>203</v>
-      </c>
-      <c r="Q26" s="24" t="s">
-        <v>205</v>
-      </c>
-      <c r="R26" t="s">
-        <v>232</v>
-      </c>
       <c r="S26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="T26" s="24" t="s">
         <v>180</v>
       </c>
       <c r="U26" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="V26" t="s">
+        <v>203</v>
+      </c>
+      <c r="W26" t="s">
         <v>204</v>
       </c>
-      <c r="W26" t="s">
-        <v>205</v>
-      </c>
       <c r="X26" s="24" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y26" s="24" t="s">
         <v>204</v>
-      </c>
-      <c r="Y26" s="24" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" s="30" t="s">
-        <v>302</v>
-      </c>
-      <c r="B29" s="27" t="s">
+        <v>301</v>
+      </c>
+      <c r="B29" s="28" t="s">
         <v>140</v>
       </c>
       <c r="C29" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="D29" t="s">
         <v>249</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>250</v>
       </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>251</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="H29" s="13" t="s">
         <v>252</v>
       </c>
-      <c r="G29" s="12" t="s">
-        <v>282</v>
-      </c>
-      <c r="H29" s="13" t="s">
+      <c r="I29" s="12" t="s">
         <v>253</v>
       </c>
-      <c r="I29" s="12" t="s">
+      <c r="J29" s="13" t="s">
         <v>254</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="L29" s="7" t="s">
         <v>255</v>
       </c>
-      <c r="L29" s="7" t="s">
+      <c r="M29" s="7" t="s">
         <v>256</v>
       </c>
-      <c r="M29" s="7" t="s">
+      <c r="N29" t="s">
         <v>257</v>
       </c>
-      <c r="N29" t="s">
+      <c r="O29" t="s">
         <v>258</v>
       </c>
-      <c r="O29" t="s">
+      <c r="P29" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="Q29" s="7" t="s">
         <v>259</v>
       </c>
-      <c r="P29" s="7" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q29" s="7" t="s">
+      <c r="R29" t="s">
+        <v>257</v>
+      </c>
+      <c r="S29" t="s">
         <v>260</v>
       </c>
-      <c r="R29" t="s">
-        <v>258</v>
-      </c>
-      <c r="S29" t="s">
-        <v>261</v>
-      </c>
       <c r="T29" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="U29" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="30"/>
-      <c r="B30" s="27"/>
+      <c r="B30" s="28"/>
       <c r="C30" s="25" t="s">
+        <v>261</v>
+      </c>
+      <c r="D30" t="s">
         <v>262</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>263</v>
       </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
         <v>264</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="G30" s="12" t="s">
+      <c r="H30" s="13" t="s">
         <v>266</v>
       </c>
-      <c r="H30" s="13" t="s">
+      <c r="I30" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="I30" s="12" t="s">
+      <c r="J30" s="13" t="s">
         <v>268</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="L30" s="7" t="s">
         <v>269</v>
       </c>
-      <c r="L30" s="7" t="s">
+      <c r="M30" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="M30" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="N30" t="s">
         <v>43</v>
       </c>
       <c r="O30" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="P30" s="7" t="s">
         <v>46</v>
       </c>
       <c r="Q30" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="R30" t="s">
         <v>45</v>
       </c>
       <c r="S30" t="s">
+        <v>272</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="U30" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="T30" s="7" t="s">
-        <v>270</v>
-      </c>
-      <c r="U30" s="7" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="31" spans="1:25" x14ac:dyDescent="0.35">
@@ -3124,58 +3125,58 @@
         <v>141</v>
       </c>
       <c r="C31" s="25" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D31" t="s">
+        <v>274</v>
+      </c>
+      <c r="E31" t="s">
         <v>275</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
         <v>276</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="H31" s="13" t="s">
         <v>278</v>
       </c>
-      <c r="H31" s="13" t="s">
+      <c r="I31" s="12" t="s">
         <v>279</v>
       </c>
-      <c r="I31" s="12" t="s">
+      <c r="J31" s="13" t="s">
         <v>280</v>
       </c>
-      <c r="J31" s="13" t="s">
-        <v>281</v>
-      </c>
       <c r="L31" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="M31" s="7" t="s">
         <v>283</v>
       </c>
-      <c r="M31" s="7" t="s">
+      <c r="N31" t="s">
         <v>284</v>
       </c>
-      <c r="N31" t="s">
+      <c r="O31" t="s">
         <v>285</v>
       </c>
-      <c r="O31" t="s">
-        <v>286</v>
-      </c>
       <c r="P31" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q31" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="Q31" s="7" t="s">
-        <v>286</v>
-      </c>
       <c r="R31" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="S31" t="s">
         <v>103</v>
       </c>
       <c r="T31" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="U31" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="32" spans="1:25" x14ac:dyDescent="0.35">
@@ -3187,70 +3188,70 @@
         <v>140</v>
       </c>
       <c r="C33" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D33" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E33" t="s">
+        <v>302</v>
+      </c>
+      <c r="F33" t="s">
         <v>303</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" s="18" t="s">
         <v>304</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="H33" s="20" t="s">
         <v>305</v>
       </c>
-      <c r="H33" s="20" t="s">
+      <c r="I33" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="I33" s="22" t="s">
+      <c r="J33" s="4" t="s">
         <v>307</v>
       </c>
-      <c r="J33" s="4" t="s">
+      <c r="K33" s="18" t="s">
+        <v>311</v>
+      </c>
+      <c r="L33" s="20" t="s">
         <v>308</v>
       </c>
-      <c r="K33" s="18" t="s">
-        <v>312</v>
-      </c>
-      <c r="L33" s="20" t="s">
+      <c r="M33" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="M33" s="22" t="s">
+      <c r="N33" s="4" t="s">
         <v>310</v>
-      </c>
-      <c r="N33" s="4" t="s">
-        <v>311</v>
       </c>
       <c r="P33" s="24" t="s">
         <v>102</v>
       </c>
       <c r="Q33" s="24" t="s">
+        <v>312</v>
+      </c>
+      <c r="R33" t="s">
         <v>313</v>
       </c>
-      <c r="R33" t="s">
+      <c r="S33" t="s">
         <v>314</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" s="24" t="s">
+        <v>313</v>
+      </c>
+      <c r="U33" s="24" t="s">
         <v>315</v>
-      </c>
-      <c r="T33" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="U33" s="24" t="s">
-        <v>316</v>
       </c>
       <c r="V33" t="s">
         <v>102</v>
       </c>
       <c r="W33" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="X33" s="24" t="s">
         <v>102</v>
       </c>
       <c r="Y33" s="24" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.35">
@@ -3259,74 +3260,84 @@
         <v>141</v>
       </c>
       <c r="C34" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D34" t="s">
+        <v>287</v>
+      </c>
+      <c r="E34" t="s">
         <v>288</v>
       </c>
-      <c r="E34" t="s">
+      <c r="F34" t="s">
         <v>289</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" s="18" t="s">
         <v>290</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="H34" s="20" t="s">
         <v>291</v>
       </c>
-      <c r="H34" s="20" t="s">
+      <c r="I34" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="J34" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="J34" s="4" t="s">
+      <c r="K34" s="18" t="s">
+        <v>295</v>
+      </c>
+      <c r="L34" s="20" t="s">
         <v>294</v>
       </c>
-      <c r="K34" s="18" t="s">
+      <c r="M34" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="L34" s="20" t="s">
-        <v>295</v>
-      </c>
-      <c r="M34" s="22" t="s">
+      <c r="N34" s="4" t="s">
         <v>297</v>
       </c>
-      <c r="N34" s="4" t="s">
+      <c r="P34" s="24" t="s">
+        <v>286</v>
+      </c>
+      <c r="Q34" s="24" t="s">
         <v>298</v>
       </c>
-      <c r="P34" s="24" t="s">
-        <v>287</v>
-      </c>
-      <c r="Q34" s="24" t="s">
+      <c r="R34" t="s">
         <v>299</v>
-      </c>
-      <c r="R34" t="s">
-        <v>300</v>
       </c>
       <c r="S34" t="s">
         <v>104</v>
       </c>
       <c r="T34" s="24" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="U34" s="24" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V34" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="W34" t="s">
         <v>104</v>
       </c>
       <c r="X34" s="24" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="Y34" s="24" t="s">
         <v>104</v>
       </c>
     </row>
+    <row r="59" spans="7:14" x14ac:dyDescent="0.35">
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+      <c r="I59" s="11"/>
+      <c r="J59" s="11"/>
+      <c r="K59" s="26"/>
+      <c r="L59" s="26"/>
+      <c r="M59" s="26"/>
+      <c r="N59" s="26"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="22">
     <mergeCell ref="A2:A26"/>
     <mergeCell ref="B29:B30"/>
     <mergeCell ref="A29:A34"/>
@@ -3343,6 +3354,7 @@
     <mergeCell ref="B5:B16"/>
     <mergeCell ref="D4:J4"/>
     <mergeCell ref="D8:J8"/>
+    <mergeCell ref="K59:N59"/>
     <mergeCell ref="P2:Q2"/>
     <mergeCell ref="R2:S2"/>
     <mergeCell ref="V22:W22"/>

</xml_diff>